<commit_message>
Añadido soporte para texto plano
</commit_message>
<xml_diff>
--- a/src/test/resources/test.xlsx
+++ b/src/test/resources/test.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27510"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/herminio/Git/citizens0/src/test/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eduardomartinez/Dropbox/Practica/ASW/citizensLoader3b/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15480"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14500"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -430,7 +430,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Añadidos los primeros comandos, la clase para encriptar, eliminadas algunas cosas y añadidas otras
</commit_message>
<xml_diff>
--- a/src/test/resources/test.xlsx
+++ b/src/test/resources/test.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eduardomartinez/Dropbox/Practica/ASW/citizensLoader3b/src/test/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Seila\Desktop\ASW\citizensLoader3b\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14500"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="14505"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,18 +19,18 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
   <si>
     <t>Nombre</t>
   </si>
@@ -96,12 +96,27 @@
   </si>
   <si>
     <t>Dirección postal</t>
+  </si>
+  <si>
+    <t>Seila</t>
+  </si>
+  <si>
+    <t>Khayat Prada</t>
+  </si>
+  <si>
+    <t>porqueestonova@joder.com</t>
+  </si>
+  <si>
+    <t>Deberia Formatear :)</t>
+  </si>
+  <si>
+    <t>34234239P</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -427,20 +442,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="23.5" customWidth="1"/>
-    <col min="4" max="4" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.1640625" customWidth="1"/>
+    <col min="1" max="3" width="23.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -463,7 +478,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -486,7 +501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -509,7 +524,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -530,6 +545,29 @@
       </c>
       <c r="G4" s="1" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="2">
+        <v>35079</v>
+      </c>
+      <c r="E5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -537,8 +575,9 @@
     <hyperlink ref="C2" r:id="rId1"/>
     <hyperlink ref="C3" r:id="rId2"/>
     <hyperlink ref="C4" r:id="rId3"/>
+    <hyperlink ref="C5" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Cambios en dbupdate, pequeños cambios para usar bien el dbupdate, cambio del fichero excel al que venia por defecto...
</commit_message>
<xml_diff>
--- a/src/test/resources/test.xlsx
+++ b/src/test/resources/test.xlsx
@@ -1,25 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/herminio/Git/citizens0/src/test/resources/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15990" windowHeight="7365"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15480"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -97,7 +101,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -423,20 +427,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="23.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.140625" customWidth="1"/>
+    <col min="1" max="3" width="23.5" customWidth="1"/>
+    <col min="4" max="4" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -459,7 +463,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -482,7 +486,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -505,7 +509,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -528,7 +532,6 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>

</xml_diff>